<commit_message>
Added search in google xaml file
</commit_message>
<xml_diff>
--- a/DynamicTableContent.xlsx
+++ b/DynamicTableContent.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <x:si>
     <x:t>Company</x:t>
   </x:si>
@@ -31,289 +31,298 @@
     <x:t>% Change</x:t>
   </x:si>
   <x:si>
+    <x:t>Dewan Housing</x:t>
+  </x:si>
+  <x:si>
+    <x:t>A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>813.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>348.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 9.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kirloskar Oil Engine</x:t>
+  </x:si>
+  <x:si>
+    <x:t>170.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>985</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 8.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kansai Nerolac Paint</x:t>
+  </x:si>
+  <x:si>
+    <x:t>341.8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>478.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 5.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>673.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>852.8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 5.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Power Finance Co</x:t>
+  </x:si>
+  <x:si>
+    <x:t>782.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>653</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 8.8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vakrangee</x:t>
+  </x:si>
+  <x:si>
+    <x:t>623</x:t>
+  </x:si>
+  <x:si>
+    <x:t>310.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 6.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hero MotoCorp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>677.6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>881</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gujarat Narmada Vall</x:t>
+  </x:si>
+  <x:si>
+    <x:t>600.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>34.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 5.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IL&amp;FS Transportation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>671.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>322.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 2.7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NIIT Technologies</x:t>
+  </x:si>
+  <x:si>
+    <x:t>795.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>348.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 2.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Apollo Hospitals</x:t>
+  </x:si>
+  <x:si>
+    <x:t>879.6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>96.8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 3.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>621</x:t>
+  </x:si>
+  <x:si>
+    <x:t>821.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 6.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>187.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>36.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 8.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Navin Fluorine Inter</x:t>
+  </x:si>
+  <x:si>
+    <x:t>516.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 9.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IIFL Holdings</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>432.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 9.7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Punj. NationlBak</x:t>
+  </x:si>
+  <x:si>
+    <x:t>574.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>955.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 4.6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Chennai Petro.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>828</x:t>
+  </x:si>
+  <x:si>
+    <x:t>364.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 8.7</x:t>
+  </x:si>
+  <x:si>
     <x:t>UCO Bank</x:t>
   </x:si>
   <x:si>
-    <x:t>A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>183.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>137.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 6.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Escorts Ltd.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>107.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>738.9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 8.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gujarat Narmada Vall</x:t>
-  </x:si>
-  <x:si>
-    <x:t>805.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>323.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 8.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Marico Ltd.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>176.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>400.8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 6.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hind. Petrol</x:t>
-  </x:si>
-  <x:si>
-    <x:t>798.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>487.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cera Sanitaryware L</x:t>
-  </x:si>
-  <x:si>
-    <x:t>689.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>452.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 4.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DCB Bank</x:t>
-  </x:si>
-  <x:si>
-    <x:t>735.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>146.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 2.8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>338.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>148.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 2.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>YES Bank Ltd.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>342.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>802</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 9.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Strides Pharma Scien</x:t>
-  </x:si>
-  <x:si>
-    <x:t>670.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>964.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 4.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>623.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>609</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 4.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Deepak Fertilisers</x:t>
-  </x:si>
-  <x:si>
-    <x:t>231.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>78.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bajaj Corp Ltd.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>189.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>66.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 7.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BEML Ltd.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>912.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>15.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 9.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vakrangee</x:t>
-  </x:si>
-  <x:si>
-    <x:t>568.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>813.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 7.8</x:t>
+    <x:t>252.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>804.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Shriram Trans.Fi</x:t>
+  </x:si>
+  <x:si>
+    <x:t>176.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>176.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 8.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mangalore Refine</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650</x:t>
+  </x:si>
+  <x:si>
+    <x:t>157.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 4.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Corporation Bank</x:t>
+  </x:si>
+  <x:si>
+    <x:t>438.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>718.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 8.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Colgate Palm.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>262.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 9.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IDFC L</x:t>
+  </x:si>
+  <x:si>
+    <x:t>596.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>225.8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 3.6</x:t>
   </x:si>
   <x:si>
     <x:t>Sun Pharma.</x:t>
   </x:si>
   <x:si>
-    <x:t>420.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>264.9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 8.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Navkar Corporation L</x:t>
-  </x:si>
-  <x:si>
-    <x:t>738.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>772.7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>35.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>724.8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Colgate Palm.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>141.7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>719.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 2.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>208.9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>693.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 2.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rashtriya Chemicals</x:t>
-  </x:si>
-  <x:si>
-    <x:t>657.7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>374.9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>924.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1000</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 3.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Power Finance Co</x:t>
-  </x:si>
-  <x:si>
-    <x:t>143.7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>217</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 8.7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jet Airways</x:t>
-  </x:si>
-  <x:si>
-    <x:t>223.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>459.8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 5.9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kansai Nerolac Paint</x:t>
-  </x:si>
-  <x:si>
-    <x:t>53.8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>694.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CESC Ltd.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>167.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>778.6</x:t>
+    <x:t>765.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>817.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 4.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>583.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>971.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PI Industries</x:t>
+  </x:si>
+  <x:si>
+    <x:t>161.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>556.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 3.8</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -740,126 +749,126 @@
     </x:row>
     <x:row r="5" spans="1:5">
       <x:c r="A5" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
+      <x:c r="D5" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="D5" s="0" t="s">
+      <x:c r="E5" s="0" t="s">
         <x:v>20</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5">
       <x:c r="A6" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
+      <x:c r="D6" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="D6" s="0" t="s">
+      <x:c r="E6" s="0" t="s">
         <x:v>24</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="s">
-        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
       <x:c r="A7" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
+      <x:c r="D7" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="D7" s="0" t="s">
+      <x:c r="E7" s="0" t="s">
         <x:v>28</x:v>
-      </x:c>
-      <x:c r="E7" s="0" t="s">
-        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5">
       <x:c r="A8" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="B8" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C8" s="0" t="s">
+      <x:c r="D8" s="0" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
       <x:c r="A9" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="D9" s="0" t="s">
+      <x:c r="E9" s="0" t="s">
         <x:v>35</x:v>
-      </x:c>
-      <x:c r="E9" s="0" t="s">
-        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
       <x:c r="A10" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C10" s="0" t="s">
+      <x:c r="D10" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="D10" s="0" t="s">
+      <x:c r="E10" s="0" t="s">
         <x:v>39</x:v>
-      </x:c>
-      <x:c r="E10" s="0" t="s">
-        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5">
       <x:c r="A11" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C11" s="0" t="s">
+      <x:c r="D11" s="0" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="D11" s="0" t="s">
+      <x:c r="E11" s="0" t="s">
         <x:v>43</x:v>
-      </x:c>
-      <x:c r="E11" s="0" t="s">
-        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
       <x:c r="A12" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
         <x:v>6</x:v>
@@ -876,109 +885,109 @@
     </x:row>
     <x:row r="13" spans="1:5">
       <x:c r="A13" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="B13" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C13" s="0" t="s">
+      <x:c r="D13" s="0" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="D13" s="0" t="s">
+      <x:c r="E13" s="0" t="s">
         <x:v>50</x:v>
-      </x:c>
-      <x:c r="E13" s="0" t="s">
-        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5">
       <x:c r="A14" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="B14" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C14" s="0" t="s">
+      <x:c r="D14" s="0" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="D14" s="0" t="s">
+      <x:c r="E14" s="0" t="s">
         <x:v>53</x:v>
-      </x:c>
-      <x:c r="E14" s="0" t="s">
-        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5">
       <x:c r="A15" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="B15" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C15" s="0" t="s">
+      <x:c r="D15" s="0" t="s">
         <x:v>56</x:v>
       </x:c>
-      <x:c r="D15" s="0" t="s">
+      <x:c r="E15" s="0" t="s">
         <x:v>57</x:v>
-      </x:c>
-      <x:c r="E15" s="0" t="s">
-        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:5">
       <x:c r="A16" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
         <x:v>59</x:v>
       </x:c>
-      <x:c r="B16" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C16" s="0" t="s">
+      <x:c r="D16" s="0" t="s">
         <x:v>60</x:v>
       </x:c>
-      <x:c r="D16" s="0" t="s">
+      <x:c r="E16" s="0" t="s">
         <x:v>61</x:v>
-      </x:c>
-      <x:c r="E16" s="0" t="s">
-        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:5">
       <x:c r="A17" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
         <x:v>63</x:v>
       </x:c>
-      <x:c r="B17" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C17" s="0" t="s">
+      <x:c r="D17" s="0" t="s">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="D17" s="0" t="s">
+      <x:c r="E17" s="0" t="s">
         <x:v>65</x:v>
-      </x:c>
-      <x:c r="E17" s="0" t="s">
-        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:5">
       <x:c r="A18" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
         <x:v>67</x:v>
       </x:c>
-      <x:c r="B18" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C18" s="0" t="s">
+      <x:c r="D18" s="0" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="D18" s="0" t="s">
+      <x:c r="E18" s="0" t="s">
         <x:v>69</x:v>
-      </x:c>
-      <x:c r="E18" s="0" t="s">
-        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:5">
       <x:c r="A19" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
         <x:v>6</x:v>
@@ -990,63 +999,63 @@
         <x:v>72</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:5">
       <x:c r="A20" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="E20" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:5">
       <x:c r="A21" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:5">
       <x:c r="A22" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="E22" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>85</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:5">
       <x:c r="A23" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
         <x:v>6</x:v>
@@ -1055,78 +1064,78 @@
         <x:v>83</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="E23" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>88</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:5">
       <x:c r="A24" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="E24" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:5">
       <x:c r="A25" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="E25" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:5">
       <x:c r="A26" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="s">
         <x:v>96</x:v>
-      </x:c>
-      <x:c r="E26" s="0" t="s">
-        <x:v>79</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:5">
       <x:c r="A27" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="D27" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="E27" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>102</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Added workflows for arguments handling
</commit_message>
<xml_diff>
--- a/DynamicTableContent.xlsx
+++ b/DynamicTableContent.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <x:si>
     <x:t>Company</x:t>
   </x:si>
@@ -31,298 +31,301 @@
     <x:t>% Change</x:t>
   </x:si>
   <x:si>
-    <x:t>Dewan Housing</x:t>
+    <x:t>Ambuja Cements Ltd.</x:t>
   </x:si>
   <x:si>
     <x:t>A</x:t>
   </x:si>
   <x:si>
-    <x:t>813.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>348.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 9.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kirloskar Oil Engine</x:t>
-  </x:si>
-  <x:si>
-    <x:t>170.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>985</x:t>
+    <x:t>452.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>515.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Navkar Corporation L</x:t>
+  </x:si>
+  <x:si>
+    <x:t>261.7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>490.8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 2.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Marico Ltd.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>44.8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>562.1</x:t>
   </x:si>
   <x:si>
     <x:t>+ 8.3</x:t>
   </x:si>
   <x:si>
-    <x:t>Kansai Nerolac Paint</x:t>
-  </x:si>
-  <x:si>
-    <x:t>341.8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>478.1</x:t>
+    <x:t>BEML Ltd.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>290.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>89.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 3.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Navin Fluorine Inter</x:t>
+  </x:si>
+  <x:si>
+    <x:t>439.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>460.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 4.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jet Airways</x:t>
+  </x:si>
+  <x:si>
+    <x:t>502.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>736.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 6.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Time Technoplast Ltd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>929.6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>68.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 2.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CESC Ltd.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>465.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>822.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 3.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NIIT Technologies</x:t>
+  </x:si>
+  <x:si>
+    <x:t>300.7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>668.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cera Sanitaryware L</x:t>
+  </x:si>
+  <x:si>
+    <x:t>64</x:t>
+  </x:si>
+  <x:si>
+    <x:t>163.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 5.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Corporation Bank</x:t>
+  </x:si>
+  <x:si>
+    <x:t>727</x:t>
+  </x:si>
+  <x:si>
+    <x:t>173.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 5.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>69.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>959.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 6.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IIFL Holdings</x:t>
+  </x:si>
+  <x:si>
+    <x:t>257.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>296.7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 6.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JaiprakashAssociates</x:t>
+  </x:si>
+  <x:si>
+    <x:t>73.6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>175.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 9.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Quess Corp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>367.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>461.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 2.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>111.7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>536.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 7.7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Coffee Day Enterpris</x:t>
+  </x:si>
+  <x:si>
+    <x:t>775.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 2.7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kwality</x:t>
+  </x:si>
+  <x:si>
+    <x:t>739.7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>965.6</x:t>
   </x:si>
   <x:si>
     <x:t>+ 5.9</x:t>
   </x:si>
   <x:si>
-    <x:t>673.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>852.8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 5.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Power Finance Co</x:t>
-  </x:si>
-  <x:si>
-    <x:t>782.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>653</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 8.8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vakrangee</x:t>
-  </x:si>
-  <x:si>
-    <x:t>623</x:t>
-  </x:si>
-  <x:si>
-    <x:t>310.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 6.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hero MotoCorp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>677.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>881</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gujarat Narmada Vall</x:t>
-  </x:si>
-  <x:si>
-    <x:t>600.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>34.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 5.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IL&amp;FS Transportation</x:t>
-  </x:si>
-  <x:si>
-    <x:t>671.9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>322.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 2.7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NIIT Technologies</x:t>
-  </x:si>
-  <x:si>
-    <x:t>795.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>348.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 2.2</x:t>
-  </x:si>
-  <x:si>
     <x:t>Apollo Hospitals</x:t>
   </x:si>
   <x:si>
-    <x:t>879.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>96.8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 3.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>621</x:t>
-  </x:si>
-  <x:si>
-    <x:t>821.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 6.9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>187.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>36.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 8.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Navin Fluorine Inter</x:t>
-  </x:si>
-  <x:si>
-    <x:t>516.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>27.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 9.9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IIFL Holdings</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19.9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>432.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 9.7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Punj. NationlBak</x:t>
-  </x:si>
-  <x:si>
-    <x:t>574.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>955.9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 4.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Chennai Petro.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>828</x:t>
-  </x:si>
-  <x:si>
-    <x:t>364.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 8.7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UCO Bank</x:t>
-  </x:si>
-  <x:si>
-    <x:t>252.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>804.9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Shriram Trans.Fi</x:t>
-  </x:si>
-  <x:si>
-    <x:t>176.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>176.9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 8.9</x:t>
+    <x:t>777.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>376</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 9.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ICICI Pru Life</x:t>
+  </x:si>
+  <x:si>
+    <x:t>550.5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>802.8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jain Irrigation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>430.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>358.8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 4.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Max Financial Servic</x:t>
+  </x:si>
+  <x:si>
+    <x:t>486.8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>634.7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>210.7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>802.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 7.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HDIL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>132.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>358.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 7.3</x:t>
   </x:si>
   <x:si>
     <x:t>Mangalore Refine</x:t>
   </x:si>
   <x:si>
-    <x:t>650</x:t>
-  </x:si>
-  <x:si>
-    <x:t>157.9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 4.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Corporation Bank</x:t>
-  </x:si>
-  <x:si>
-    <x:t>438.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>718.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 8.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Colgate Palm.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>262.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 9.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IDFC L</x:t>
-  </x:si>
-  <x:si>
-    <x:t>596.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>225.8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 3.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sun Pharma.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>765.1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>817.9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 4.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>583.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>971.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PI Industries</x:t>
-  </x:si>
-  <x:si>
-    <x:t>161.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>556.3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>+ 3.8</x:t>
+    <x:t>171.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>595.7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 2.1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Asian Paints Ltd.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>384.7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>618.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>+ 4.4</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -749,291 +752,291 @@
     </x:row>
     <x:row r="5" spans="1:5">
       <x:c r="A5" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5">
       <x:c r="A6" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
       <x:c r="A7" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5">
       <x:c r="A8" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
       <x:c r="A9" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
       <x:c r="A10" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5">
       <x:c r="A11" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
       <x:c r="A12" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5">
       <x:c r="A13" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5">
       <x:c r="A14" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5">
       <x:c r="A15" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:5">
       <x:c r="A16" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>64</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:5">
       <x:c r="A17" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="E17" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:5">
       <x:c r="A18" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E18" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:5">
       <x:c r="A19" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:5">
       <x:c r="A20" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="E20" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:5">
       <x:c r="A21" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:5">
@@ -1061,52 +1064,52 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="E23" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:5">
       <x:c r="A24" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
         <x:v>89</x:v>
       </x:c>
-      <x:c r="B24" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C24" s="0" t="s">
+      <x:c r="D24" s="0" t="s">
         <x:v>90</x:v>
       </x:c>
-      <x:c r="D24" s="0" t="s">
+      <x:c r="E24" s="0" t="s">
         <x:v>91</x:v>
-      </x:c>
-      <x:c r="E24" s="0" t="s">
-        <x:v>92</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:5">
       <x:c r="A25" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
         <x:v>93</x:v>
       </x:c>
-      <x:c r="B25" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C25" s="0" t="s">
+      <x:c r="D25" s="0" t="s">
         <x:v>94</x:v>
       </x:c>
-      <x:c r="D25" s="0" t="s">
+      <x:c r="E25" s="0" t="s">
         <x:v>95</x:v>
-      </x:c>
-      <x:c r="E25" s="0" t="s">
-        <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:5">
       <x:c r="A26" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
         <x:v>6</x:v>
@@ -1118,24 +1121,24 @@
         <x:v>98</x:v>
       </x:c>
       <x:c r="E26" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>99</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:5">
       <x:c r="A27" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="D27" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="E27" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>